<commit_message>
Add Chrome DevTools and update selenium libraries
Add Chrome DevTools and update selenium libraries
</commit_message>
<xml_diff>
--- a/HomePageTestCasesandData.xlsx
+++ b/HomePageTestCasesandData.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DE3ED3-22CE-4C58-87F6-9CAA6E9DA9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B89AD6-215B-456B-89EF-910DAB8E0A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="selectActionTest1" sheetId="2" r:id="rId1"/>
-    <sheet name="selectActionTest" sheetId="3" r:id="rId2"/>
+    <sheet name="selectActionTest" sheetId="3" r:id="rId1"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Keyword</t>
   </si>
@@ -45,9 +44,6 @@
   </si>
   <si>
     <t>TestCase</t>
-  </si>
-  <si>
-    <t>Inpatient Ward</t>
   </si>
   <si>
     <t>Iteration1</t>
@@ -534,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E88B823-AB0D-4107-B578-734CE6DE5A43}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF0B568-C35A-473C-ABEE-344328F1B6E7}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,12 +560,12 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -582,86 +578,6 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>[1]Objects!$B$8</f>
-        <v>referenceapplication-registrationapp-registerPatient-homepageLink-referenceapplication-registrationapp-registerPatient-homepageLink-extension</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>[1]Objects!$C$8</f>
-        <v>id</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>[1]Objects!$B$16</f>
-        <v>givenName</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>[1]Objects!$C$16</f>
-        <v>name</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF0B568-C35A-473C-ABEE-344328F1B6E7}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="str">
         <f>[1]Objects!$B$6</f>
         <v>coreapps-activeVisitsHomepageLink-coreapps-activeVisitsHomepageLink-extension</v>
       </c>
@@ -674,7 +590,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>[1]Objects!$B$15</f>
@@ -689,7 +605,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -708,14 +624,12 @@
         <f>[1]Objects!$C$8</f>
         <v>id</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]Objects!$B$16</f>

</xml_diff>